<commit_message>
Laatste versie kaart NL
</commit_message>
<xml_diff>
--- a/Drive/Logboeken/Logboek Felix.xlsx
+++ b/Drive/Logboeken/Logboek Felix.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="53">
   <si>
     <t>TOTAAL</t>
   </si>
@@ -163,6 +163,18 @@
   </si>
   <si>
     <t>SQL leren</t>
+  </si>
+  <si>
+    <t>Layout update: custom checkboxes / buttons en andere dingen</t>
+  </si>
+  <si>
+    <t>Code bestuderen en bugfixen</t>
+  </si>
+  <si>
+    <t>Skype + verder werken layout + rivieren in nieuwe kaart verwerken</t>
+  </si>
+  <si>
+    <t>Verder werken aan app</t>
   </si>
 </sst>
 </file>
@@ -599,10 +611,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I56"/>
+  <dimension ref="A1:I60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A57" sqref="A57"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B60" sqref="B60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -627,8 +639,8 @@
         <v>0</v>
       </c>
       <c r="H1" s="5">
-        <f>(SUM(C20,C38,C56))</f>
-        <v>113</v>
+        <f>(SUM(C20,C38,C60))</f>
+        <v>131</v>
       </c>
       <c r="I1" s="4"/>
     </row>
@@ -1053,7 +1065,7 @@
         <v>2.5</v>
       </c>
       <c r="C25" s="5">
-        <f>SUM(B25,C24)</f>
+        <f t="shared" ref="C25:C38" si="0">SUM(B25,C24)</f>
         <v>4.5</v>
       </c>
       <c r="D25" s="3" t="s">
@@ -1073,7 +1085,7 @@
         <v>2</v>
       </c>
       <c r="C26" s="5">
-        <f>SUM(B26,C25)</f>
+        <f t="shared" si="0"/>
         <v>6.5</v>
       </c>
       <c r="D26" s="3" t="s">
@@ -1093,7 +1105,7 @@
         <v>4</v>
       </c>
       <c r="C27" s="5">
-        <f>SUM(B27,C26)</f>
+        <f t="shared" si="0"/>
         <v>10.5</v>
       </c>
       <c r="D27" s="3" t="s">
@@ -1113,7 +1125,7 @@
         <v>3</v>
       </c>
       <c r="C28" s="5">
-        <f>SUM(B28,C27)</f>
+        <f t="shared" si="0"/>
         <v>13.5</v>
       </c>
       <c r="D28" s="3" t="s">
@@ -1133,7 +1145,7 @@
         <v>2</v>
       </c>
       <c r="C29" s="5">
-        <f>SUM(B29,C28)</f>
+        <f t="shared" si="0"/>
         <v>15.5</v>
       </c>
       <c r="D29" s="15" t="s">
@@ -1153,7 +1165,7 @@
         <v>3</v>
       </c>
       <c r="C30" s="5">
-        <f>SUM(B30,C29)</f>
+        <f t="shared" si="0"/>
         <v>18.5</v>
       </c>
       <c r="D30" s="3" t="s">
@@ -1173,7 +1185,7 @@
         <v>3</v>
       </c>
       <c r="C31" s="5">
-        <f>SUM(B31,C30)</f>
+        <f t="shared" si="0"/>
         <v>21.5</v>
       </c>
       <c r="D31" s="3" t="s">
@@ -1193,7 +1205,7 @@
         <v>4</v>
       </c>
       <c r="C32" s="5">
-        <f>SUM(B32,C31)</f>
+        <f t="shared" si="0"/>
         <v>25.5</v>
       </c>
       <c r="D32" s="3" t="s">
@@ -1213,7 +1225,7 @@
         <v>3.5</v>
       </c>
       <c r="C33" s="5">
-        <f>SUM(B33,C32)</f>
+        <f t="shared" si="0"/>
         <v>29</v>
       </c>
       <c r="D33" s="3" t="s">
@@ -1233,7 +1245,7 @@
         <v>3.5</v>
       </c>
       <c r="C34" s="5">
-        <f>SUM(B34,C33)</f>
+        <f t="shared" si="0"/>
         <v>32.5</v>
       </c>
       <c r="D34" s="3" t="s">
@@ -1253,7 +1265,7 @@
         <v>4</v>
       </c>
       <c r="C35" s="5">
-        <f>SUM(B35,C34)</f>
+        <f t="shared" si="0"/>
         <v>36.5</v>
       </c>
       <c r="D35" s="3" t="s">
@@ -1273,7 +1285,7 @@
         <v>3.5</v>
       </c>
       <c r="C36" s="5">
-        <f>SUM(B36,C35)</f>
+        <f t="shared" si="0"/>
         <v>40</v>
       </c>
       <c r="D36" s="3" t="s">
@@ -1293,7 +1305,7 @@
         <v>3</v>
       </c>
       <c r="C37" s="5">
-        <f>SUM(B37,C36)</f>
+        <f t="shared" si="0"/>
         <v>43</v>
       </c>
       <c r="D37" s="3" t="s">
@@ -1313,7 +1325,7 @@
         <v>4</v>
       </c>
       <c r="C38" s="5">
-        <f>SUM(B38,C37)</f>
+        <f t="shared" si="0"/>
         <v>47</v>
       </c>
       <c r="D38" s="3" t="s">
@@ -1416,7 +1428,7 @@
         <v>5</v>
       </c>
       <c r="C44" s="4">
-        <f t="shared" ref="C44:C58" si="0">(SUM(C43,B44))</f>
+        <f t="shared" ref="C44:C60" si="1">(SUM(C43,B44))</f>
         <v>7</v>
       </c>
       <c r="D44" s="6" t="s">
@@ -1431,7 +1443,7 @@
         <v>1</v>
       </c>
       <c r="C45" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="D45" t="s">
@@ -1446,7 +1458,7 @@
         <v>2</v>
       </c>
       <c r="C46" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="D46" s="13" t="s">
@@ -1461,7 +1473,7 @@
         <v>2</v>
       </c>
       <c r="C47" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="D47" s="13" t="s">
@@ -1476,7 +1488,7 @@
         <v>2</v>
       </c>
       <c r="C48" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>14</v>
       </c>
       <c r="D48" s="13" t="s">
@@ -1491,7 +1503,7 @@
         <v>4</v>
       </c>
       <c r="C49" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>18</v>
       </c>
       <c r="D49" s="13" t="s">
@@ -1506,7 +1518,7 @@
         <v>1.5</v>
       </c>
       <c r="C50" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>19.5</v>
       </c>
       <c r="D50" s="13" t="s">
@@ -1521,7 +1533,7 @@
         <v>1.5</v>
       </c>
       <c r="C51" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>21</v>
       </c>
       <c r="D51" s="13" t="s">
@@ -1536,7 +1548,7 @@
         <v>2</v>
       </c>
       <c r="C52" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>23</v>
       </c>
       <c r="D52" s="13" t="s">
@@ -1551,7 +1563,7 @@
         <v>2</v>
       </c>
       <c r="C53" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>25</v>
       </c>
       <c r="D53" t="s">
@@ -1566,7 +1578,7 @@
         <v>2</v>
       </c>
       <c r="C54" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>27</v>
       </c>
       <c r="D54" s="13" t="s">
@@ -1581,7 +1593,7 @@
         <v>3</v>
       </c>
       <c r="C55" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>30</v>
       </c>
       <c r="D55" t="s">
@@ -1596,11 +1608,71 @@
         <v>6</v>
       </c>
       <c r="C56" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>36</v>
       </c>
       <c r="D56" t="s">
         <v>40</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>22</v>
+      </c>
+      <c r="B57">
+        <v>1.5</v>
+      </c>
+      <c r="C57" s="4">
+        <f t="shared" si="1"/>
+        <v>37.5</v>
+      </c>
+      <c r="D57" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>23</v>
+      </c>
+      <c r="B58">
+        <v>4</v>
+      </c>
+      <c r="C58" s="4">
+        <f t="shared" si="1"/>
+        <v>41.5</v>
+      </c>
+      <c r="D58" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>24</v>
+      </c>
+      <c r="B59">
+        <v>6.5</v>
+      </c>
+      <c r="C59" s="4">
+        <f t="shared" si="1"/>
+        <v>48</v>
+      </c>
+      <c r="D59" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>25</v>
+      </c>
+      <c r="B60">
+        <v>6</v>
+      </c>
+      <c r="C60" s="4">
+        <f t="shared" si="1"/>
+        <v>54</v>
+      </c>
+      <c r="D60" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>